<commit_message>
render termino de version entregable
</commit_message>
<xml_diff>
--- a/assets/tabulados/R10_responsable_horario.xlsx
+++ b/assets/tabulados/R10_responsable_horario.xlsx
@@ -6,8 +6,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Responsable_horario" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Responsable_horario'!$A$1:$Q$17</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -624,8 +627,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="#,##0"/>
+    <numFmt numFmtId="167" formatCode="0.0&quot;%&quot;"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -633,16 +639,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F4E79"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -650,12 +672,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -945,912 +1001,934 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="0" tabSelected="true">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="11.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="7.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="7.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="13.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="15.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="17.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="19.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="9.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="10.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="12.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="22.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="8.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="8.71" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="8.71" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="8.71" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="8.71" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="8.71" hidden="0" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q9" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="Q12" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q13" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q14" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="P15" t="s">
+      <c r="P15" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="Q15" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="P16" t="s">
+      <c r="P16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16" s="2" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q17" s="2" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>